<commit_message>
Se modifica ejemplo descriptiva
</commit_message>
<xml_diff>
--- a/Dataset/EjemploDescriptiva.xlsx
+++ b/Dataset/EjemploDescriptiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E9D4F33-00DC-4C32-BA6B-96EC048C01FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62F6DDD-8300-497D-B6A1-4E2148C9ADDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFDC961B-5D18-4380-85F8-DC89FCDD9440}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t>Municipio</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Muy insatisfecho</t>
+  </si>
+  <si>
+    <t>Estrato</t>
   </si>
 </sst>
 </file>
@@ -446,494 +449,557 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C7EBEB-8A26-4683-A315-7C2C44753A4F}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
         <v>17</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>1.77</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>66</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1635100</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
         <v>27</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>1.65</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>90</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1752500</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>18</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>1.57</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>66</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1858400</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
         <v>22</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>1.84</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>87</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2131400</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>20</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>1.86</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>89</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1874800</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
         <v>22</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>1.74</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>90</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>2933100</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
         <v>20</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>1.91</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>79</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1637200</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
         <v>27</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>1.77</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>88</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>1171200</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
         <v>20</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>1.58</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>61</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2574700</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>16</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
         <v>39</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>1.81</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>70</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>2739000</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
         <v>16</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>1.69</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>78</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>2887800</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>19</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
         <v>40</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>1.93</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>83</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>2559600</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>16</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
         <v>26</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>1.93</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>91</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>1906600</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>18</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
         <v>21</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>1.87</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>61</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>1299700</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>18</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
         <v>23</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>1.6</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>84</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>1950900</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>19</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
         <v>40</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>1.91</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>76</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>2131900</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>18</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
         <v>31</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>1.79</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>66</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>1085400</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>19</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
       <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
         <v>40</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>1.6</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>67</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>1182200</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>19</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
         <v>32</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>1.6</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>88</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>2541900</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>19</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
         <v>33</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>1.81</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>65</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>1333200</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>16</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>